<commit_message>
Add test for calculated grocery amount
</commit_message>
<xml_diff>
--- a/data/groceries.xlsx
+++ b/data/groceries.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joema\projects\JMRecipes\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BCE131E-27D4-46B8-AC90-DCFAE2B0F389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD3E3EEB-2C14-4FD6-8231-4A180681E0DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="17715" windowHeight="10545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="224">
   <si>
     <t>name</t>
   </si>
@@ -690,6 +690,24 @@
   </si>
   <si>
     <t>https://www.walmart.com/ip/Fresh-Roma-Tomato-Each/44390944?athbdg=L1200&amp;from=/search</t>
+  </si>
+  <si>
+    <t>liter</t>
+  </si>
+  <si>
+    <t>test volume</t>
+  </si>
+  <si>
+    <t>test weight</t>
+  </si>
+  <si>
+    <t>test other</t>
+  </si>
+  <si>
+    <t>test count</t>
+  </si>
+  <si>
+    <t>loaf</t>
   </si>
 </sst>
 </file>
@@ -1028,13 +1046,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P94"/>
+  <dimension ref="A1:P98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E36" sqref="E36"/>
+      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1098,446 +1116,414 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C2" t="s">
-        <v>148</v>
-      </c>
-      <c r="D2" s="2">
-        <v>1.39</v>
-      </c>
-      <c r="K2" s="1">
+        <v>219</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1">
         <v>1</v>
       </c>
-      <c r="L2">
-        <v>64</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>15</v>
-      </c>
-      <c r="O2">
-        <v>2</v>
-      </c>
+      <c r="F2" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="2">
-        <v>2.98</v>
-      </c>
-      <c r="I3" s="1">
+        <v>220</v>
+      </c>
+      <c r="G3" s="1">
         <v>1</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L3">
-        <v>150</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>30</v>
-      </c>
-      <c r="O3">
-        <v>12</v>
-      </c>
+      <c r="H3" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>100</v>
-      </c>
-      <c r="B4" t="s">
-        <v>99</v>
-      </c>
-      <c r="C4" t="s">
-        <v>149</v>
-      </c>
-      <c r="D4" s="2">
-        <v>4.79</v>
-      </c>
-      <c r="G4" s="1">
-        <v>3</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="K4" s="1">
-        <v>5</v>
-      </c>
-      <c r="L4">
-        <v>300</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4" s="1">
-        <v>80</v>
-      </c>
-      <c r="O4" s="1">
-        <v>15</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="I4" s="1">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C5" t="s">
-        <v>150</v>
-      </c>
-      <c r="D5" s="2">
-        <v>1.48</v>
+      <c r="A5" t="s">
+        <v>222</v>
       </c>
       <c r="K5" s="1">
         <v>1</v>
       </c>
-      <c r="L5">
-        <v>46</v>
-      </c>
-      <c r="M5">
-        <v>0.5</v>
-      </c>
-      <c r="N5">
-        <v>9</v>
-      </c>
-      <c r="O5">
-        <v>1.5</v>
-      </c>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B6" t="s">
         <v>99</v>
       </c>
       <c r="C6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D6" s="2">
-        <v>2.2799999999999998</v>
-      </c>
-      <c r="G6" s="1">
-        <v>10</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>8</v>
+        <v>1.39</v>
+      </c>
+      <c r="K6" s="1">
+        <v>1</v>
       </c>
       <c r="L6">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="M6">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="N6">
-        <v>5.8</v>
+        <v>15</v>
       </c>
       <c r="O6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>103</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
         <v>99</v>
       </c>
       <c r="C7" t="s">
-        <v>152</v>
+        <v>34</v>
       </c>
       <c r="D7" s="2">
-        <v>0.88</v>
+        <v>2.98</v>
       </c>
       <c r="I7" s="1">
         <v>1</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>153</v>
+        <v>14</v>
       </c>
       <c r="L7">
-        <v>10</v>
+        <v>150</v>
       </c>
       <c r="M7">
         <v>0</v>
       </c>
       <c r="N7">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="O7">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B8" t="s">
         <v>99</v>
       </c>
       <c r="C8" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="D8" s="2">
-        <v>1.18</v>
+        <v>4.79</v>
+      </c>
+      <c r="G8" s="1">
+        <v>3</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>114</v>
       </c>
       <c r="K8" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L8">
-        <v>64</v>
+        <v>300</v>
       </c>
       <c r="M8">
         <v>0</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="1">
+        <v>80</v>
+      </c>
+      <c r="O8" s="1">
         <v>15</v>
       </c>
-      <c r="O8">
-        <v>2</v>
-      </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>105</v>
+      <c r="A9" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="B9" t="s">
         <v>99</v>
       </c>
       <c r="C9" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D9" s="2">
-        <v>0.96</v>
+        <v>1.48</v>
       </c>
       <c r="K9" s="1">
         <v>1</v>
       </c>
+      <c r="L9">
+        <v>46</v>
+      </c>
+      <c r="M9">
+        <v>0.5</v>
+      </c>
+      <c r="N9">
+        <v>9</v>
+      </c>
+      <c r="O9">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B10" t="s">
         <v>99</v>
       </c>
-      <c r="D10" s="2"/>
+      <c r="C10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D10" s="2">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="G10" s="1">
+        <v>10</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L10">
+        <v>50</v>
+      </c>
+      <c r="M10">
+        <v>0.6</v>
+      </c>
+      <c r="N10">
+        <v>5.8</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>216</v>
+        <v>103</v>
       </c>
       <c r="B11" t="s">
         <v>99</v>
       </c>
       <c r="C11" t="s">
-        <v>217</v>
+        <v>152</v>
       </c>
       <c r="D11" s="2">
-        <v>0.27</v>
-      </c>
-      <c r="K11" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="I11" s="1">
         <v>1</v>
       </c>
+      <c r="J11" s="1" t="s">
+        <v>153</v>
+      </c>
       <c r="L11">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M11">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="N11">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="O11">
-        <v>0.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B12" t="s">
         <v>99</v>
       </c>
       <c r="C12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D12" s="2">
-        <v>0.88</v>
-      </c>
-      <c r="I12" s="1">
+        <v>1.18</v>
+      </c>
+      <c r="K12" s="1">
         <v>1</v>
       </c>
-      <c r="J12" s="1" t="s">
-        <v>153</v>
+      <c r="L12">
+        <v>64</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>15</v>
+      </c>
+      <c r="O12">
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>105</v>
       </c>
       <c r="B13" t="s">
         <v>99</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>155</v>
       </c>
       <c r="D13" s="2">
-        <v>0.38</v>
+        <v>0.96</v>
       </c>
       <c r="K13" s="1">
         <v>1</v>
       </c>
-      <c r="L13">
-        <v>20</v>
-      </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="N13">
-        <v>7</v>
-      </c>
-      <c r="O13">
-        <v>0</v>
-      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>106</v>
       </c>
       <c r="B14" t="s">
         <v>99</v>
       </c>
-      <c r="C14" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="2">
-        <v>0.93</v>
-      </c>
-      <c r="K14" s="1">
-        <v>1</v>
-      </c>
-      <c r="L14">
-        <v>33</v>
-      </c>
-      <c r="M14">
-        <v>1</v>
-      </c>
-      <c r="N14">
-        <v>6</v>
-      </c>
-      <c r="O14">
-        <v>2</v>
-      </c>
+      <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>86</v>
+        <v>216</v>
       </c>
       <c r="B15" t="s">
         <v>99</v>
       </c>
-      <c r="D15" s="2"/>
+      <c r="C15" t="s">
+        <v>217</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0.27</v>
+      </c>
+      <c r="K15" s="1">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>11</v>
+      </c>
+      <c r="M15">
+        <v>0.1</v>
+      </c>
+      <c r="N15">
+        <v>2.5</v>
+      </c>
+      <c r="O15">
+        <v>0.6</v>
+      </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>201</v>
+        <v>107</v>
       </c>
       <c r="B16" t="s">
         <v>99</v>
       </c>
       <c r="C16" t="s">
-        <v>202</v>
+        <v>156</v>
       </c>
       <c r="D16" s="2">
-        <v>3.48</v>
-      </c>
-      <c r="G16" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="L16">
-        <v>480</v>
-      </c>
-      <c r="M16">
-        <v>0</v>
-      </c>
-      <c r="N16">
-        <v>120</v>
-      </c>
-      <c r="O16">
-        <v>12</v>
+        <v>0.88</v>
+      </c>
+      <c r="I16" s="1">
+        <v>1</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B17" t="s">
         <v>99</v>
       </c>
       <c r="C17" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="D17" s="2">
-        <v>0.57999999999999996</v>
+        <v>0.38</v>
       </c>
       <c r="K17" s="1">
         <v>1</v>
       </c>
       <c r="L17">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="M17">
         <v>0</v>
       </c>
       <c r="N17">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O17">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="B18" t="s">
         <v>99</v>
       </c>
       <c r="C18" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="D18" s="2">
-        <v>0.96</v>
+        <v>0.93</v>
+      </c>
+      <c r="K18" s="1">
+        <v>1</v>
       </c>
       <c r="L18">
-        <v>112</v>
+        <v>33</v>
       </c>
       <c r="M18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N18">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="O18">
         <v>2</v>
@@ -1545,325 +1531,311 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>86</v>
       </c>
       <c r="B19" t="s">
         <v>99</v>
       </c>
-      <c r="C19" t="s">
-        <v>54</v>
-      </c>
-      <c r="D19" s="2">
-        <v>0.27</v>
-      </c>
-      <c r="K19" s="1">
-        <v>1</v>
-      </c>
-      <c r="L19">
-        <v>90</v>
-      </c>
-      <c r="M19">
-        <v>0</v>
-      </c>
-      <c r="N19">
-        <v>15</v>
-      </c>
-      <c r="O19">
-        <v>1</v>
-      </c>
+      <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>108</v>
+        <v>201</v>
       </c>
       <c r="B20" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="C20" t="s">
-        <v>157</v>
+        <v>202</v>
       </c>
       <c r="D20" s="2">
-        <v>2.48</v>
-      </c>
-      <c r="E20" s="1">
-        <v>5.5</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>24</v>
+        <v>3.48</v>
       </c>
       <c r="G20" s="1">
-        <v>32</v>
+        <v>1.5</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>8</v>
+        <v>114</v>
       </c>
       <c r="L20">
-        <v>770</v>
+        <v>480</v>
       </c>
       <c r="M20">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="N20">
-        <v>176</v>
+        <v>120</v>
       </c>
       <c r="O20">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" t="s">
+        <v>99</v>
+      </c>
+      <c r="C21" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="K21" s="1">
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <v>17</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
         <v>5</v>
       </c>
-      <c r="B21" t="s">
-        <v>109</v>
-      </c>
-      <c r="C21" t="s">
-        <v>55</v>
-      </c>
-      <c r="D21" s="2">
-        <v>7.84</v>
-      </c>
-      <c r="E21" s="1">
-        <v>10</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L21">
-        <v>1000</v>
-      </c>
-      <c r="M21">
-        <v>15</v>
-      </c>
-      <c r="N21">
-        <v>240</v>
-      </c>
       <c r="O21">
-        <v>0</v>
-      </c>
-      <c r="P21" t="s">
-        <v>110</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B22" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="C22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D22" s="2"/>
-      <c r="G22" s="1">
+        <v>53</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0.96</v>
+      </c>
+      <c r="L22">
+        <v>112</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
         <v>26</v>
       </c>
-      <c r="H22" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L22">
-        <v>630</v>
-      </c>
-      <c r="M22">
-        <v>0</v>
-      </c>
-      <c r="N22">
-        <v>162</v>
-      </c>
       <c r="O22">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>111</v>
+        <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="C23" t="s">
-        <v>113</v>
+        <v>54</v>
       </c>
       <c r="D23" s="2">
-        <v>7.52</v>
-      </c>
-      <c r="G23" s="1">
+        <v>0.27</v>
+      </c>
+      <c r="K23" s="1">
         <v>1</v>
       </c>
-      <c r="H23" s="1" t="s">
-        <v>114</v>
-      </c>
       <c r="L23">
-        <v>560</v>
+        <v>90</v>
       </c>
       <c r="M23">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="N23">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="O23">
-        <v>92</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B24" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C24" t="s">
-        <v>116</v>
+        <v>157</v>
       </c>
       <c r="D24" s="2">
-        <v>13.59</v>
+        <v>2.48</v>
+      </c>
+      <c r="E24" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="G24" s="1">
-        <v>4.5999999999999996</v>
+        <v>32</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="K24" s="1">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="L24">
-        <v>2525</v>
+        <v>770</v>
       </c>
       <c r="M24">
-        <v>86</v>
+        <v>5.5</v>
       </c>
       <c r="N24">
-        <v>0</v>
+        <v>176</v>
       </c>
       <c r="O24">
-        <v>410</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>117</v>
+        <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C25" t="s">
-        <v>118</v>
+        <v>55</v>
       </c>
       <c r="D25" s="2">
-        <v>5.49</v>
-      </c>
-      <c r="G25" s="1">
-        <v>1</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>114</v>
+        <v>7.84</v>
+      </c>
+      <c r="E25" s="1">
+        <v>10</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="L25">
-        <v>1020</v>
+        <v>1000</v>
       </c>
       <c r="M25">
-        <v>78</v>
+        <v>15</v>
       </c>
       <c r="N25">
-        <v>24</v>
+        <v>240</v>
       </c>
       <c r="O25">
-        <v>60</v>
+        <v>0</v>
+      </c>
+      <c r="P25" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>119</v>
+        <v>60</v>
       </c>
       <c r="B26" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C26" t="s">
-        <v>120</v>
-      </c>
-      <c r="D26" s="2">
-        <v>12.07</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="D26" s="2"/>
       <c r="G26" s="1">
-        <v>1.1599999999999999</v>
+        <v>26</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="K26" s="1">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="L26">
+        <v>630</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>162</v>
+      </c>
+      <c r="O26">
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="B27" t="s">
         <v>112</v>
       </c>
       <c r="C27" t="s">
-        <v>158</v>
+        <v>113</v>
       </c>
       <c r="D27" s="2">
-        <v>5.96</v>
+        <v>7.52</v>
       </c>
       <c r="G27" s="1">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>114</v>
       </c>
       <c r="L27">
-        <v>1560</v>
+        <v>560</v>
       </c>
       <c r="M27">
-        <v>120</v>
+        <v>32</v>
       </c>
       <c r="N27">
         <v>0</v>
       </c>
       <c r="O27">
-        <v>114</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B28" t="s">
         <v>112</v>
       </c>
       <c r="C28" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="D28" s="2">
-        <v>17.66</v>
+        <v>13.59</v>
       </c>
       <c r="G28" s="1">
-        <v>2.21</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>114</v>
       </c>
       <c r="K28" s="1">
-        <v>1</v>
+        <v>16</v>
+      </c>
+      <c r="L28">
+        <v>2525</v>
+      </c>
+      <c r="M28">
+        <v>86</v>
+      </c>
+      <c r="N28">
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <v>410</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B29" t="s">
         <v>112</v>
       </c>
       <c r="C29" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D29" s="2">
-        <v>4.99</v>
+        <v>5.49</v>
       </c>
       <c r="G29" s="1">
         <v>1</v>
@@ -1871,184 +1843,193 @@
       <c r="H29" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="P29" t="s">
-        <v>125</v>
+      <c r="L29">
+        <v>1020</v>
+      </c>
+      <c r="M29">
+        <v>78</v>
+      </c>
+      <c r="N29">
+        <v>24</v>
+      </c>
+      <c r="O29">
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>90</v>
+        <v>119</v>
       </c>
       <c r="B30" t="s">
         <v>112</v>
       </c>
       <c r="C30" t="s">
-        <v>159</v>
+        <v>120</v>
       </c>
       <c r="D30" s="2">
-        <v>2.79</v>
+        <v>12.07</v>
       </c>
       <c r="G30" s="1">
-        <v>1</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="L30">
-        <v>440</v>
-      </c>
-      <c r="M30">
-        <v>10</v>
-      </c>
-      <c r="N30">
-        <v>0</v>
-      </c>
-      <c r="O30">
-        <v>92</v>
+      <c r="K30" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>126</v>
+        <v>87</v>
       </c>
       <c r="B31" t="s">
         <v>112</v>
       </c>
       <c r="C31" t="s">
-        <v>127</v>
+        <v>158</v>
       </c>
       <c r="D31" s="2">
-        <v>2.97</v>
+        <v>5.96</v>
       </c>
       <c r="G31" s="1">
-        <v>12</v>
+        <v>1.5</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>8</v>
+        <v>114</v>
       </c>
       <c r="L31">
-        <v>800</v>
+        <v>1560</v>
       </c>
       <c r="M31">
-        <v>64</v>
+        <v>120</v>
       </c>
       <c r="N31">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="O31">
-        <v>40</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B32" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="C32" t="s">
-        <v>194</v>
+        <v>122</v>
       </c>
       <c r="D32" s="2">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="E32" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="P32" t="s">
-        <v>181</v>
+        <v>17.66</v>
+      </c>
+      <c r="G32" s="1">
+        <v>2.21</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="K32" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>29</v>
+        <v>123</v>
       </c>
       <c r="B33" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="C33" t="s">
-        <v>35</v>
+        <v>124</v>
       </c>
       <c r="D33" s="2">
-        <v>2.54</v>
-      </c>
-      <c r="E33" s="1">
-        <v>83</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L33">
-        <v>0</v>
-      </c>
-      <c r="M33">
-        <v>0</v>
-      </c>
-      <c r="N33">
-        <v>0</v>
-      </c>
-      <c r="O33">
-        <v>0</v>
+        <v>4.99</v>
+      </c>
+      <c r="G33" s="1">
+        <v>1</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="P33" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>130</v>
+        <v>90</v>
       </c>
       <c r="B34" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="C34" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="D34" s="2">
-        <v>5.64</v>
-      </c>
-      <c r="E34" s="1">
+        <v>2.79</v>
+      </c>
+      <c r="G34" s="1">
         <v>1</v>
       </c>
-      <c r="F34" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="P34" t="s">
-        <v>181</v>
+      <c r="H34" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="L34">
+        <v>440</v>
+      </c>
+      <c r="M34">
+        <v>10</v>
+      </c>
+      <c r="N34">
+        <v>0</v>
+      </c>
+      <c r="O34">
+        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>74</v>
+        <v>126</v>
       </c>
       <c r="B35" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="C35" t="s">
-        <v>182</v>
+        <v>127</v>
       </c>
       <c r="D35" s="2">
-        <v>2.2400000000000002</v>
-      </c>
-      <c r="E35" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="P35" t="s">
-        <v>181</v>
+        <v>2.97</v>
+      </c>
+      <c r="G35" s="1">
+        <v>12</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L35">
+        <v>800</v>
+      </c>
+      <c r="M35">
+        <v>64</v>
+      </c>
+      <c r="N35">
+        <v>8</v>
+      </c>
+      <c r="O35">
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B36" t="s">
         <v>129</v>
       </c>
       <c r="C36" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
       <c r="D36" s="2">
         <v>1.1200000000000001</v>
@@ -2065,42 +2046,51 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>132</v>
+        <v>29</v>
       </c>
       <c r="B37" t="s">
         <v>129</v>
       </c>
       <c r="C37" t="s">
-        <v>184</v>
+        <v>35</v>
       </c>
       <c r="D37" s="2">
-        <v>1.1200000000000001</v>
+        <v>2.54</v>
       </c>
       <c r="E37" s="1">
-        <v>0.5</v>
+        <v>83</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="P37" t="s">
-        <v>181</v>
+        <v>17</v>
+      </c>
+      <c r="L37">
+        <v>0</v>
+      </c>
+      <c r="M37">
+        <v>0</v>
+      </c>
+      <c r="N37">
+        <v>0</v>
+      </c>
+      <c r="O37">
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>77</v>
+        <v>130</v>
       </c>
       <c r="B38" t="s">
         <v>129</v>
       </c>
       <c r="C38" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D38" s="2">
-        <v>1.1200000000000001</v>
+        <v>5.64</v>
       </c>
       <c r="E38" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>180</v>
@@ -2111,22 +2101,36 @@
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B39" t="s">
         <v>129</v>
       </c>
-      <c r="D39" s="2"/>
+      <c r="C39" t="s">
+        <v>182</v>
+      </c>
+      <c r="D39" s="2">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="E39" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="P39" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B40" t="s">
         <v>129</v>
       </c>
       <c r="C40" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D40" s="2">
         <v>1.1200000000000001</v>
@@ -2143,19 +2147,19 @@
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B41" t="s">
         <v>129</v>
       </c>
       <c r="C41" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D41" s="2">
-        <v>3.98</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="E41" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>180</v>
@@ -2166,16 +2170,16 @@
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>135</v>
+        <v>77</v>
       </c>
       <c r="B42" t="s">
         <v>129</v>
       </c>
       <c r="C42" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D42" s="2">
-        <v>1.28</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="E42" s="1">
         <v>0.5</v>
@@ -2189,39 +2193,25 @@
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>136</v>
+        <v>80</v>
       </c>
       <c r="B43" t="s">
         <v>129</v>
       </c>
-      <c r="C43" t="s">
-        <v>189</v>
-      </c>
-      <c r="D43" s="2">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="E43" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="P43" t="s">
-        <v>181</v>
-      </c>
+      <c r="D43" s="2"/>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B44" t="s">
         <v>129</v>
       </c>
       <c r="C44" t="s">
-        <v>160</v>
+        <v>186</v>
       </c>
       <c r="D44" s="2">
-        <v>1.18</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="E44" s="1">
         <v>0.5</v>
@@ -2235,19 +2225,19 @@
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B45" t="s">
         <v>129</v>
       </c>
       <c r="C45" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D45" s="2">
-        <v>3.78</v>
+        <v>3.98</v>
       </c>
       <c r="E45" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>180</v>
@@ -2258,16 +2248,16 @@
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>88</v>
+        <v>135</v>
       </c>
       <c r="B46" t="s">
         <v>129</v>
       </c>
       <c r="C46" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D46" s="2">
-        <v>2.42</v>
+        <v>1.28</v>
       </c>
       <c r="E46" s="1">
         <v>0.5</v>
@@ -2281,569 +2271,550 @@
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>211</v>
+        <v>136</v>
       </c>
       <c r="B47" t="s">
         <v>129</v>
       </c>
-      <c r="C47" s="4" t="s">
-        <v>212</v>
+      <c r="C47" t="s">
+        <v>189</v>
       </c>
       <c r="D47" s="2">
-        <v>0.89</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="E47" s="1">
-        <v>16</v>
+        <v>0.5</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L47">
-        <v>120</v>
-      </c>
-      <c r="M47">
-        <v>0</v>
-      </c>
-      <c r="N47">
-        <v>24</v>
-      </c>
-      <c r="O47">
-        <v>0</v>
+        <v>180</v>
+      </c>
+      <c r="P47" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>137</v>
+      </c>
+      <c r="B48" t="s">
+        <v>129</v>
+      </c>
+      <c r="C48" t="s">
+        <v>160</v>
+      </c>
+      <c r="D48" s="2">
+        <v>1.18</v>
+      </c>
+      <c r="E48" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="P48" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>138</v>
+      </c>
+      <c r="B49" t="s">
+        <v>129</v>
+      </c>
+      <c r="C49" t="s">
+        <v>190</v>
+      </c>
+      <c r="D49" s="2">
+        <v>3.78</v>
+      </c>
+      <c r="E49" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="P49" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>88</v>
+      </c>
+      <c r="B50" t="s">
+        <v>129</v>
+      </c>
+      <c r="C50" t="s">
+        <v>191</v>
+      </c>
+      <c r="D50" s="2">
+        <v>2.42</v>
+      </c>
+      <c r="E50" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="P50" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>211</v>
+      </c>
+      <c r="B51" t="s">
+        <v>129</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="D51" s="2">
+        <v>0.89</v>
+      </c>
+      <c r="E51" s="1">
+        <v>16</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L51">
+        <v>120</v>
+      </c>
+      <c r="M51">
+        <v>0</v>
+      </c>
+      <c r="N51">
+        <v>24</v>
+      </c>
+      <c r="O51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>139</v>
-      </c>
-      <c r="B48" t="s">
-        <v>140</v>
-      </c>
-      <c r="C48" t="s">
-        <v>145</v>
-      </c>
-      <c r="D48" s="2">
-        <v>1.73</v>
-      </c>
-      <c r="K48" s="1">
-        <v>18</v>
-      </c>
-      <c r="L48">
-        <v>1260</v>
-      </c>
-      <c r="M48">
-        <v>90</v>
-      </c>
-      <c r="N48">
-        <v>0</v>
-      </c>
-      <c r="O48">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>141</v>
-      </c>
-      <c r="B49" t="s">
-        <v>140</v>
-      </c>
-      <c r="C49" t="s">
-        <v>146</v>
-      </c>
-      <c r="D49" s="2">
-        <v>2.48</v>
-      </c>
-      <c r="E49" s="1">
-        <v>1</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="L49">
-        <v>240</v>
-      </c>
-      <c r="M49">
-        <v>128</v>
-      </c>
-      <c r="N49">
-        <v>192</v>
-      </c>
-      <c r="O49">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>46</v>
-      </c>
-      <c r="B50" t="s">
-        <v>140</v>
-      </c>
-      <c r="C50" t="s">
-        <v>47</v>
-      </c>
-      <c r="D50" s="2">
-        <v>5.48</v>
-      </c>
-      <c r="E50" s="1">
-        <v>182</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L50">
-        <v>1820</v>
-      </c>
-      <c r="M50">
-        <v>136</v>
-      </c>
-      <c r="N50">
-        <v>0</v>
-      </c>
-      <c r="O50">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>25</v>
-      </c>
-      <c r="B51" t="s">
-        <v>140</v>
-      </c>
-      <c r="C51" t="s">
-        <v>48</v>
-      </c>
-      <c r="D51" s="2">
-        <v>3.68</v>
-      </c>
-      <c r="E51" s="1">
-        <v>32</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L51">
-        <v>3200</v>
-      </c>
-      <c r="M51">
-        <v>352</v>
-      </c>
-      <c r="N51">
-        <v>0</v>
-      </c>
-      <c r="O51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>58</v>
       </c>
       <c r="B52" t="s">
         <v>140</v>
       </c>
       <c r="C52" t="s">
-        <v>59</v>
+        <v>145</v>
       </c>
       <c r="D52" s="2">
-        <v>2.78</v>
-      </c>
-      <c r="E52" s="1">
-        <v>32</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>20</v>
+        <v>1.73</v>
+      </c>
+      <c r="K52" s="1">
+        <v>18</v>
       </c>
       <c r="L52">
-        <v>1600</v>
+        <v>1260</v>
       </c>
       <c r="M52">
-        <v>160</v>
+        <v>90</v>
       </c>
       <c r="N52">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="O52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B53" t="s">
         <v>140</v>
       </c>
       <c r="C53" t="s">
+        <v>146</v>
+      </c>
+      <c r="D53" s="2">
+        <v>2.48</v>
+      </c>
+      <c r="E53" s="1">
+        <v>1</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="L53">
+        <v>240</v>
+      </c>
+      <c r="M53">
+        <v>128</v>
+      </c>
+      <c r="N53">
+        <v>192</v>
+      </c>
+      <c r="O53">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>46</v>
+      </c>
+      <c r="B54" t="s">
+        <v>140</v>
+      </c>
+      <c r="C54" t="s">
+        <v>47</v>
+      </c>
+      <c r="D54" s="2">
+        <v>5.48</v>
+      </c>
+      <c r="E54" s="1">
+        <v>182</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L54">
+        <v>1820</v>
+      </c>
+      <c r="M54">
+        <v>136</v>
+      </c>
+      <c r="N54">
+        <v>0</v>
+      </c>
+      <c r="O54">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>25</v>
+      </c>
+      <c r="B55" t="s">
+        <v>140</v>
+      </c>
+      <c r="C55" t="s">
+        <v>48</v>
+      </c>
+      <c r="D55" s="2">
+        <v>3.68</v>
+      </c>
+      <c r="E55" s="1">
+        <v>32</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L55">
+        <v>3200</v>
+      </c>
+      <c r="M55">
+        <v>352</v>
+      </c>
+      <c r="N55">
+        <v>0</v>
+      </c>
+      <c r="O55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>58</v>
+      </c>
+      <c r="B56" t="s">
+        <v>140</v>
+      </c>
+      <c r="C56" t="s">
+        <v>59</v>
+      </c>
+      <c r="D56" s="2">
+        <v>2.78</v>
+      </c>
+      <c r="E56" s="1">
+        <v>32</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L56">
+        <v>1600</v>
+      </c>
+      <c r="M56">
+        <v>160</v>
+      </c>
+      <c r="N56">
+        <v>32</v>
+      </c>
+      <c r="O56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>142</v>
+      </c>
+      <c r="B57" t="s">
+        <v>140</v>
+      </c>
+      <c r="C57" t="s">
         <v>161</v>
       </c>
-      <c r="D53" s="2">
+      <c r="D57" s="2">
         <v>3.68</v>
       </c>
-      <c r="G53" s="1">
+      <c r="G57" s="1">
         <v>16</v>
-      </c>
-      <c r="H53" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L53">
-        <v>1760</v>
-      </c>
-      <c r="M53">
-        <v>144</v>
-      </c>
-      <c r="N53">
-        <v>0</v>
-      </c>
-      <c r="O53">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>39</v>
-      </c>
-      <c r="B54" t="s">
-        <v>162</v>
-      </c>
-      <c r="C54" t="s">
-        <v>40</v>
-      </c>
-      <c r="D54" s="2">
-        <v>0.78</v>
-      </c>
-      <c r="G54" s="1">
-        <v>15.5</v>
-      </c>
-      <c r="H54" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L54">
-        <v>350</v>
-      </c>
-      <c r="M54">
-        <v>0</v>
-      </c>
-      <c r="N54">
-        <v>73</v>
-      </c>
-      <c r="O54">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>78</v>
-      </c>
-      <c r="B55" t="s">
-        <v>162</v>
-      </c>
-      <c r="C55" t="s">
-        <v>163</v>
-      </c>
-      <c r="D55" s="2">
-        <v>0.78</v>
-      </c>
-      <c r="G55" s="1">
-        <v>15.5</v>
-      </c>
-      <c r="H55" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L55">
-        <v>385</v>
-      </c>
-      <c r="M55">
-        <v>3.5</v>
-      </c>
-      <c r="N55">
-        <v>70</v>
-      </c>
-      <c r="O55">
-        <v>24.5</v>
-      </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>79</v>
-      </c>
-      <c r="B56" t="s">
-        <v>162</v>
-      </c>
-      <c r="C56" t="s">
-        <v>164</v>
-      </c>
-      <c r="D56" s="2">
-        <v>1.48</v>
-      </c>
-      <c r="G56" s="1">
-        <v>28</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L56">
-        <v>175</v>
-      </c>
-      <c r="M56">
-        <v>0</v>
-      </c>
-      <c r="N56">
-        <v>35</v>
-      </c>
-      <c r="O56">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>41</v>
-      </c>
-      <c r="B57" t="s">
-        <v>162</v>
-      </c>
-      <c r="C57" t="s">
-        <v>42</v>
-      </c>
-      <c r="D57" s="2">
-        <v>0.86</v>
-      </c>
-      <c r="E57" s="1">
-        <v>10</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G57" s="1">
-        <v>6</v>
       </c>
       <c r="H57" s="1" t="s">
         <v>8</v>
       </c>
       <c r="L57">
-        <v>150</v>
+        <v>1760</v>
       </c>
       <c r="M57">
-        <v>0</v>
+        <v>144</v>
       </c>
       <c r="N57">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="O57">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="B58" t="s">
         <v>162</v>
       </c>
       <c r="C58" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="D58" s="2">
-        <v>0.68</v>
+        <v>0.78</v>
       </c>
       <c r="G58" s="1">
-        <v>10.5</v>
+        <v>15.5</v>
       </c>
       <c r="H58" s="1" t="s">
         <v>8</v>
       </c>
       <c r="L58">
-        <v>250</v>
+        <v>350</v>
       </c>
       <c r="M58">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="N58">
-        <v>25</v>
+        <v>73</v>
       </c>
       <c r="O58">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="B59" t="s">
         <v>162</v>
       </c>
       <c r="C59" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D59" s="2">
-        <v>0.64</v>
+        <v>0.78</v>
       </c>
       <c r="G59" s="1">
-        <v>14.5</v>
+        <v>15.5</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>8</v>
       </c>
       <c r="L59">
-        <v>52.5</v>
+        <v>385</v>
       </c>
       <c r="M59">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="N59">
+        <v>70</v>
+      </c>
+      <c r="O59">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>79</v>
+      </c>
+      <c r="B60" t="s">
+        <v>162</v>
+      </c>
+      <c r="C60" t="s">
+        <v>164</v>
+      </c>
+      <c r="D60" s="2">
+        <v>1.48</v>
+      </c>
+      <c r="G60" s="1">
+        <v>28</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L60">
+        <v>175</v>
+      </c>
+      <c r="M60">
+        <v>0</v>
+      </c>
+      <c r="N60">
+        <v>35</v>
+      </c>
+      <c r="O60">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>41</v>
+      </c>
+      <c r="B61" t="s">
+        <v>162</v>
+      </c>
+      <c r="C61" t="s">
+        <v>42</v>
+      </c>
+      <c r="D61" s="2">
+        <v>0.86</v>
+      </c>
+      <c r="E61" s="1">
+        <v>10</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G61" s="1">
+        <v>6</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L61">
+        <v>150</v>
+      </c>
+      <c r="M61">
+        <v>0</v>
+      </c>
+      <c r="N61">
+        <v>30</v>
+      </c>
+      <c r="O61">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>62</v>
+      </c>
+      <c r="B62" t="s">
+        <v>162</v>
+      </c>
+      <c r="C62" t="s">
+        <v>63</v>
+      </c>
+      <c r="D62" s="2">
+        <v>0.68</v>
+      </c>
+      <c r="G62" s="1">
         <v>10.5</v>
       </c>
-      <c r="O59">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>82</v>
-      </c>
-      <c r="B60" t="s">
-        <v>166</v>
-      </c>
-      <c r="C60" t="s">
-        <v>195</v>
-      </c>
-      <c r="D60" s="2">
-        <v>13.99</v>
-      </c>
-      <c r="E60" s="1">
-        <v>144</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="L60">
-        <v>1872</v>
-      </c>
-      <c r="M60">
-        <v>0</v>
-      </c>
-      <c r="N60">
-        <v>158</v>
-      </c>
-      <c r="O60">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>83</v>
-      </c>
-      <c r="B61" t="s">
-        <v>167</v>
-      </c>
-      <c r="D61" s="2"/>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>49</v>
-      </c>
-      <c r="B62" t="s">
-        <v>167</v>
-      </c>
-      <c r="C62" t="s">
-        <v>50</v>
-      </c>
-      <c r="D62" s="2">
-        <v>1.37</v>
-      </c>
-      <c r="E62" s="1">
-        <v>4</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>24</v>
+      <c r="H62" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="L62">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="M62">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="N62">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="O62">
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B63" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C63" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D63" s="2">
-        <v>33.5</v>
-      </c>
-      <c r="I63" s="1">
-        <v>20</v>
-      </c>
-      <c r="J63" s="1" t="s">
-        <v>169</v>
+        <v>0.64</v>
+      </c>
+      <c r="G63" s="1">
+        <v>14.5</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="L63">
-        <v>3400</v>
+        <v>52.5</v>
       </c>
       <c r="M63">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="N63">
-        <v>140</v>
+        <v>10.5</v>
       </c>
       <c r="O63">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="B64" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C64" t="s">
-        <v>65</v>
+        <v>195</v>
       </c>
       <c r="D64" s="2">
-        <v>2.94</v>
+        <v>13.99</v>
       </c>
       <c r="E64" s="1">
-        <v>36</v>
+        <v>144</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G64" s="1">
-        <v>6</v>
-      </c>
-      <c r="H64" s="1" t="s">
-        <v>8</v>
+        <v>196</v>
       </c>
       <c r="L64">
-        <v>960</v>
+        <v>1872</v>
       </c>
       <c r="M64">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="N64">
-        <v>96</v>
+        <v>158</v>
       </c>
       <c r="O64">
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="B65" t="s">
         <v>167</v>
@@ -2852,308 +2823,337 @@
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>97</v>
+        <v>49</v>
       </c>
       <c r="B66" t="s">
         <v>167</v>
       </c>
       <c r="C66" t="s">
-        <v>170</v>
+        <v>50</v>
       </c>
       <c r="D66" s="2">
-        <v>4.24</v>
+        <v>1.37</v>
       </c>
       <c r="E66" s="1">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G66" s="1">
         <v>24</v>
       </c>
-      <c r="H66" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="L66">
-        <v>3600</v>
+        <v>40</v>
       </c>
       <c r="M66">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="N66">
-        <v>450</v>
+        <v>0</v>
       </c>
       <c r="O66">
-        <v>45</v>
+        <v>2</v>
       </c>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
       <c r="B67" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C67" t="s">
-        <v>71</v>
+        <v>168</v>
       </c>
       <c r="D67" s="2">
-        <v>2.98</v>
-      </c>
-      <c r="K67" s="1">
-        <v>8</v>
+        <v>33.5</v>
+      </c>
+      <c r="I67" s="1">
+        <v>20</v>
+      </c>
+      <c r="J67" s="1" t="s">
+        <v>169</v>
       </c>
       <c r="L67">
-        <v>1760</v>
+        <v>3400</v>
       </c>
       <c r="M67">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="N67">
-        <v>320</v>
+        <v>140</v>
       </c>
       <c r="O67">
-        <v>56</v>
+        <v>600</v>
       </c>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="B68" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C68" t="s">
-        <v>143</v>
+        <v>65</v>
       </c>
       <c r="D68" s="2">
-        <v>3.46</v>
-      </c>
-      <c r="I68" s="1">
-        <v>15</v>
-      </c>
-      <c r="J68" s="1" t="s">
-        <v>144</v>
+        <v>2.94</v>
+      </c>
+      <c r="E68" s="1">
+        <v>36</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G68" s="1">
+        <v>6</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="L68">
-        <v>1650</v>
+        <v>960</v>
       </c>
       <c r="M68">
-        <v>22.5</v>
+        <v>72</v>
       </c>
       <c r="N68">
-        <v>300</v>
+        <v>96</v>
       </c>
       <c r="O68">
-        <v>60</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>22</v>
+        <v>95</v>
       </c>
       <c r="B69" t="s">
-        <v>172</v>
-      </c>
-      <c r="C69" t="s">
-        <v>23</v>
-      </c>
-      <c r="D69" s="2">
-        <v>1.77</v>
-      </c>
-      <c r="E69" s="1">
-        <v>4</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L69">
-        <v>800</v>
-      </c>
-      <c r="M69">
-        <v>0</v>
-      </c>
-      <c r="N69">
-        <v>168</v>
-      </c>
-      <c r="O69">
-        <v>24</v>
-      </c>
+        <v>167</v>
+      </c>
+      <c r="D69" s="2"/>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>18</v>
+        <v>97</v>
       </c>
       <c r="B70" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C70" t="s">
-        <v>19</v>
+        <v>170</v>
       </c>
       <c r="D70" s="2">
-        <v>4.62</v>
+        <v>4.24</v>
       </c>
       <c r="E70" s="1">
-        <v>500</v>
+        <v>45</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="G70" s="1">
+        <v>24</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="L70">
-        <v>495</v>
+        <v>3600</v>
       </c>
       <c r="M70">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="N70">
-        <v>99</v>
+        <v>450</v>
       </c>
       <c r="O70">
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>15</v>
+        <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C71" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D71" s="2">
-        <v>4.9800000000000004</v>
-      </c>
-      <c r="E71" s="1">
-        <v>181</v>
-      </c>
-      <c r="F71" s="1" t="s">
-        <v>17</v>
+        <v>2.98</v>
+      </c>
+      <c r="K71" s="1">
+        <v>8</v>
       </c>
       <c r="L71">
-        <v>905</v>
+        <v>1760</v>
       </c>
       <c r="M71">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="N71">
-        <v>181</v>
+        <v>320</v>
       </c>
       <c r="O71">
-        <v>0</v>
+        <v>56</v>
       </c>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="B72" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C72" t="s">
-        <v>173</v>
+        <v>143</v>
       </c>
       <c r="D72" s="2">
-        <v>2.16</v>
-      </c>
-      <c r="E72" s="1">
-        <v>443</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>21</v>
+        <v>3.46</v>
+      </c>
+      <c r="I72" s="1">
+        <v>15</v>
+      </c>
+      <c r="J72" s="1" t="s">
+        <v>144</v>
       </c>
       <c r="L72">
-        <v>3000</v>
+        <v>1650</v>
       </c>
       <c r="M72">
-        <v>330</v>
+        <v>22.5</v>
       </c>
       <c r="N72">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="O72">
-        <v>0</v>
+        <v>60</v>
       </c>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>73</v>
+        <v>22</v>
       </c>
       <c r="B73" t="s">
         <v>172</v>
       </c>
       <c r="C73" t="s">
-        <v>174</v>
+        <v>23</v>
       </c>
       <c r="D73" s="2">
-        <v>7.42</v>
+        <v>1.77</v>
       </c>
       <c r="E73" s="1">
-        <v>754</v>
+        <v>4</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="L73">
-        <v>6000</v>
+        <v>800</v>
       </c>
       <c r="M73">
-        <v>700</v>
+        <v>0</v>
       </c>
       <c r="N73">
-        <v>0</v>
+        <v>168</v>
       </c>
       <c r="O73">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>75</v>
+        <v>18</v>
       </c>
       <c r="B74" t="s">
         <v>172</v>
       </c>
-      <c r="D74" s="2"/>
+      <c r="C74" t="s">
+        <v>19</v>
+      </c>
+      <c r="D74" s="2">
+        <v>4.62</v>
+      </c>
+      <c r="E74" s="1">
+        <v>500</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L74">
+        <v>495</v>
+      </c>
+      <c r="M74">
+        <v>0</v>
+      </c>
+      <c r="N74">
+        <v>99</v>
+      </c>
+      <c r="O74">
+        <v>0</v>
+      </c>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>76</v>
+        <v>15</v>
       </c>
       <c r="B75" t="s">
         <v>172</v>
       </c>
-      <c r="D75" s="2"/>
+      <c r="C75" t="s">
+        <v>16</v>
+      </c>
+      <c r="D75" s="2">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="E75" s="1">
+        <v>181</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L75">
+        <v>905</v>
+      </c>
+      <c r="M75">
+        <v>0</v>
+      </c>
+      <c r="N75">
+        <v>181</v>
+      </c>
+      <c r="O75">
+        <v>0</v>
+      </c>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B76" t="s">
         <v>172</v>
       </c>
       <c r="C76" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D76" s="2">
-        <v>1</v>
+        <v>2.16</v>
       </c>
       <c r="E76" s="1">
-        <v>296</v>
+        <v>443</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>21</v>
       </c>
       <c r="L76">
-        <v>295</v>
+        <v>3000</v>
       </c>
       <c r="M76">
-        <v>0</v>
+        <v>330</v>
       </c>
       <c r="N76">
-        <v>59</v>
+        <v>0</v>
       </c>
       <c r="O76">
         <v>0</v>
@@ -3161,31 +3161,31 @@
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B77" t="s">
         <v>172</v>
       </c>
       <c r="C77" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D77" s="2">
-        <v>2.36</v>
+        <v>7.42</v>
       </c>
       <c r="E77" s="1">
-        <v>709</v>
+        <v>754</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>21</v>
       </c>
       <c r="L77">
-        <v>2400</v>
+        <v>6000</v>
       </c>
       <c r="M77">
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="N77">
-        <v>624</v>
+        <v>0</v>
       </c>
       <c r="O77">
         <v>0</v>
@@ -3193,244 +3193,201 @@
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="B78" t="s">
         <v>172</v>
       </c>
-      <c r="C78" t="s">
-        <v>57</v>
-      </c>
-      <c r="D78" s="2">
-        <v>1.37</v>
-      </c>
-      <c r="E78" s="1">
-        <v>4</v>
-      </c>
-      <c r="F78" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G78" s="1">
-        <v>32</v>
-      </c>
-      <c r="H78" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L78">
-        <v>40</v>
-      </c>
-      <c r="M78">
-        <v>0</v>
-      </c>
-      <c r="N78">
-        <v>0</v>
-      </c>
-      <c r="O78">
-        <v>4</v>
-      </c>
+      <c r="D78" s="2"/>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="B79" t="s">
         <v>172</v>
       </c>
-      <c r="C79" t="s">
-        <v>67</v>
-      </c>
-      <c r="D79" s="2">
-        <v>2.34</v>
-      </c>
-      <c r="E79" s="1">
-        <v>18.75</v>
-      </c>
-      <c r="F79" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L79">
-        <v>8250</v>
-      </c>
-      <c r="M79">
-        <v>0</v>
-      </c>
-      <c r="N79">
-        <v>1725</v>
-      </c>
-      <c r="O79">
-        <v>225</v>
-      </c>
+      <c r="D79" s="2"/>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="B80" t="s">
         <v>172</v>
       </c>
-      <c r="D80" s="2"/>
+      <c r="C80" t="s">
+        <v>175</v>
+      </c>
+      <c r="D80" s="2">
+        <v>1</v>
+      </c>
+      <c r="E80" s="1">
+        <v>296</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L80">
+        <v>295</v>
+      </c>
+      <c r="M80">
+        <v>0</v>
+      </c>
+      <c r="N80">
+        <v>59</v>
+      </c>
+      <c r="O80">
+        <v>0</v>
+      </c>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="B81" t="s">
         <v>172</v>
       </c>
-      <c r="D81" s="2"/>
+      <c r="C81" t="s">
+        <v>177</v>
+      </c>
+      <c r="D81" s="2">
+        <v>2.36</v>
+      </c>
+      <c r="E81" s="1">
+        <v>709</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L81">
+        <v>2400</v>
+      </c>
+      <c r="M81">
+        <v>0</v>
+      </c>
+      <c r="N81">
+        <v>624</v>
+      </c>
+      <c r="O81">
+        <v>0</v>
+      </c>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>96</v>
+        <v>56</v>
       </c>
       <c r="B82" t="s">
         <v>172</v>
       </c>
       <c r="C82" t="s">
-        <v>215</v>
+        <v>57</v>
       </c>
       <c r="D82" s="2">
-        <v>3.24</v>
+        <v>1.37</v>
       </c>
       <c r="E82" s="1">
-        <v>554</v>
+        <v>4</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
+      </c>
+      <c r="G82" s="1">
+        <v>32</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="L82">
-        <v>6810</v>
+        <v>40</v>
       </c>
       <c r="M82">
         <v>0</v>
       </c>
       <c r="N82">
-        <v>1816</v>
+        <v>0</v>
       </c>
       <c r="O82">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="B83" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C83" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="D83" s="2">
-        <v>1.28</v>
-      </c>
-      <c r="I83" s="1">
-        <v>1</v>
-      </c>
-      <c r="J83" s="1" t="s">
-        <v>68</v>
+        <v>2.34</v>
+      </c>
+      <c r="E83" s="1">
+        <v>18.75</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="L83">
-        <v>480</v>
+        <v>8250</v>
       </c>
       <c r="M83">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="N83">
-        <v>84</v>
+        <v>1725</v>
       </c>
       <c r="O83">
-        <v>12</v>
+        <v>225</v>
       </c>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>37</v>
+        <v>93</v>
       </c>
       <c r="B84" t="s">
-        <v>176</v>
-      </c>
-      <c r="C84" t="s">
-        <v>38</v>
-      </c>
-      <c r="D84" s="2">
-        <v>5.97</v>
-      </c>
-      <c r="E84" s="1">
-        <v>12.5</v>
-      </c>
-      <c r="F84" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L84">
-        <v>9000</v>
-      </c>
-      <c r="M84">
-        <v>0</v>
-      </c>
-      <c r="N84">
-        <v>1750</v>
-      </c>
-      <c r="O84">
-        <v>150</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="D84" s="2"/>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B85" t="s">
-        <v>176</v>
-      </c>
-      <c r="C85" t="s">
-        <v>203</v>
-      </c>
-      <c r="D85" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="G85" s="1">
-        <v>16</v>
-      </c>
-      <c r="H85" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L85">
-        <v>1600</v>
-      </c>
-      <c r="M85">
-        <v>8</v>
-      </c>
-      <c r="N85">
-        <v>328</v>
-      </c>
-      <c r="O85">
-        <v>56</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="D85" s="2"/>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>192</v>
+        <v>96</v>
+      </c>
+      <c r="B86" t="s">
+        <v>172</v>
       </c>
       <c r="C86" t="s">
-        <v>193</v>
+        <v>215</v>
       </c>
       <c r="D86" s="2">
-        <v>4.28</v>
+        <v>3.24</v>
       </c>
       <c r="E86" s="1">
-        <v>38</v>
+        <v>554</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>17</v>
       </c>
       <c r="L86">
-        <v>380</v>
+        <v>6810</v>
       </c>
       <c r="M86">
         <v>0</v>
       </c>
       <c r="N86">
-        <v>38</v>
+        <v>1816</v>
       </c>
       <c r="O86">
         <v>0</v>
@@ -3438,194 +3395,319 @@
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>198</v>
+        <v>12</v>
       </c>
       <c r="B87" t="s">
-        <v>197</v>
-      </c>
-      <c r="D87" s="2"/>
+        <v>176</v>
+      </c>
+      <c r="C87" t="s">
+        <v>36</v>
+      </c>
+      <c r="D87" s="2">
+        <v>1.28</v>
+      </c>
+      <c r="I87" s="1">
+        <v>1</v>
+      </c>
+      <c r="J87" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="L87">
+        <v>480</v>
+      </c>
+      <c r="M87">
+        <v>12</v>
+      </c>
+      <c r="N87">
+        <v>84</v>
+      </c>
+      <c r="O87">
+        <v>12</v>
+      </c>
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>199</v>
+        <v>37</v>
       </c>
       <c r="B88" t="s">
-        <v>197</v>
-      </c>
-      <c r="D88" s="2"/>
+        <v>176</v>
+      </c>
+      <c r="C88" t="s">
+        <v>38</v>
+      </c>
+      <c r="D88" s="2">
+        <v>5.97</v>
+      </c>
+      <c r="E88" s="1">
+        <v>12.5</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L88">
+        <v>9000</v>
+      </c>
+      <c r="M88">
+        <v>0</v>
+      </c>
+      <c r="N88">
+        <v>1750</v>
+      </c>
+      <c r="O88">
+        <v>150</v>
+      </c>
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>200</v>
+        <v>91</v>
       </c>
       <c r="B89" t="s">
-        <v>197</v>
-      </c>
-      <c r="D89" s="2"/>
+        <v>176</v>
+      </c>
+      <c r="C89" t="s">
+        <v>203</v>
+      </c>
+      <c r="D89" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="G89" s="1">
+        <v>16</v>
+      </c>
+      <c r="H89" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L89">
+        <v>1600</v>
+      </c>
+      <c r="M89">
+        <v>8</v>
+      </c>
+      <c r="N89">
+        <v>328</v>
+      </c>
+      <c r="O89">
+        <v>56</v>
+      </c>
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>204</v>
-      </c>
-      <c r="B90" t="s">
-        <v>176</v>
+        <v>192</v>
+      </c>
+      <c r="C90" t="s">
+        <v>193</v>
       </c>
       <c r="D90" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="G90" s="1">
-        <v>16</v>
-      </c>
-      <c r="H90" s="1" t="s">
-        <v>8</v>
+        <v>4.28</v>
+      </c>
+      <c r="E90" s="1">
+        <v>38</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="L90">
-        <v>1600</v>
+        <v>380</v>
       </c>
       <c r="M90">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="N90">
-        <v>328</v>
+        <v>38</v>
       </c>
       <c r="O90">
-        <v>56</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="B91" t="s">
-        <v>167</v>
-      </c>
-      <c r="C91" t="s">
-        <v>206</v>
-      </c>
-      <c r="D91" s="2">
-        <v>1.99</v>
-      </c>
-      <c r="G91" s="1">
-        <v>24</v>
-      </c>
-      <c r="H91" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L91">
-        <v>350</v>
-      </c>
-      <c r="M91">
-        <v>10</v>
-      </c>
-      <c r="N91">
-        <v>60</v>
-      </c>
-      <c r="O91">
-        <v>10</v>
-      </c>
+        <v>197</v>
+      </c>
+      <c r="D91" s="2"/>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="B92" t="s">
-        <v>171</v>
-      </c>
-      <c r="C92" t="s">
-        <v>208</v>
-      </c>
-      <c r="D92" s="2">
-        <v>2.99</v>
-      </c>
-      <c r="K92" s="1">
-        <v>8</v>
-      </c>
-      <c r="L92">
-        <v>1920</v>
-      </c>
-      <c r="M92">
-        <v>28</v>
-      </c>
-      <c r="N92">
-        <v>344</v>
-      </c>
-      <c r="O92">
-        <v>56</v>
-      </c>
+        <v>197</v>
+      </c>
+      <c r="D92" s="2"/>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="B93" t="s">
-        <v>176</v>
-      </c>
-      <c r="C93" t="s">
-        <v>210</v>
-      </c>
-      <c r="D93" s="2">
-        <v>3.98</v>
-      </c>
-      <c r="E93" s="1">
-        <v>13.5</v>
-      </c>
-      <c r="F93" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G93" s="1">
-        <v>5</v>
-      </c>
-      <c r="H93" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="L93">
-        <v>8100</v>
-      </c>
-      <c r="M93">
-        <v>81</v>
-      </c>
-      <c r="N93">
-        <v>1728</v>
-      </c>
-      <c r="O93">
-        <v>162</v>
-      </c>
+        <v>197</v>
+      </c>
+      <c r="D93" s="2"/>
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="B94" t="s">
-        <v>171</v>
-      </c>
-      <c r="C94" t="s">
-        <v>214</v>
+        <v>176</v>
       </c>
       <c r="D94" s="2">
-        <v>1.47</v>
+        <v>1.5</v>
       </c>
       <c r="G94" s="1">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H94" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I94" s="1">
-        <v>24</v>
-      </c>
-      <c r="J94" s="1" t="s">
-        <v>144</v>
-      </c>
       <c r="L94">
-        <v>1120</v>
+        <v>1600</v>
       </c>
       <c r="M94">
         <v>8</v>
       </c>
       <c r="N94">
+        <v>328</v>
+      </c>
+      <c r="O94">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>205</v>
+      </c>
+      <c r="B95" t="s">
+        <v>167</v>
+      </c>
+      <c r="C95" t="s">
+        <v>206</v>
+      </c>
+      <c r="D95" s="2">
+        <v>1.99</v>
+      </c>
+      <c r="G95" s="1">
+        <v>24</v>
+      </c>
+      <c r="H95" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L95">
+        <v>350</v>
+      </c>
+      <c r="M95">
+        <v>10</v>
+      </c>
+      <c r="N95">
+        <v>60</v>
+      </c>
+      <c r="O95">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>207</v>
+      </c>
+      <c r="B96" t="s">
+        <v>171</v>
+      </c>
+      <c r="C96" t="s">
+        <v>208</v>
+      </c>
+      <c r="D96" s="2">
+        <v>2.99</v>
+      </c>
+      <c r="K96" s="1">
+        <v>8</v>
+      </c>
+      <c r="L96">
+        <v>1920</v>
+      </c>
+      <c r="M96">
+        <v>28</v>
+      </c>
+      <c r="N96">
+        <v>344</v>
+      </c>
+      <c r="O96">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>209</v>
+      </c>
+      <c r="B97" t="s">
+        <v>176</v>
+      </c>
+      <c r="C97" t="s">
+        <v>210</v>
+      </c>
+      <c r="D97" s="2">
+        <v>3.98</v>
+      </c>
+      <c r="E97" s="1">
+        <v>13.5</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G97" s="1">
+        <v>5</v>
+      </c>
+      <c r="H97" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="L97">
+        <v>8100</v>
+      </c>
+      <c r="M97">
+        <v>81</v>
+      </c>
+      <c r="N97">
+        <v>1728</v>
+      </c>
+      <c r="O97">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>213</v>
+      </c>
+      <c r="B98" t="s">
+        <v>171</v>
+      </c>
+      <c r="C98" t="s">
+        <v>214</v>
+      </c>
+      <c r="D98" s="2">
+        <v>1.47</v>
+      </c>
+      <c r="G98" s="1">
+        <v>14</v>
+      </c>
+      <c r="H98" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I98" s="1">
+        <v>24</v>
+      </c>
+      <c r="J98" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="L98">
+        <v>1120</v>
+      </c>
+      <c r="M98">
+        <v>8</v>
+      </c>
+      <c r="N98">
         <v>184</v>
       </c>
-      <c r="O94">
+      <c r="O98">
         <v>40</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Calculates nested recipe nutrition
</commit_message>
<xml_diff>
--- a/data/groceries.xlsx
+++ b/data/groceries.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joema\projects\JMRecipes\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD3E3EEB-2C14-4FD6-8231-4A180681E0DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1552DB7F-9955-4479-A9B2-8583D759A1B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="17715" windowHeight="10545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -572,9 +572,6 @@
     <t>https://www.walmart.com/ip/Great-Value-Original-Syrup-24-oz/10315480?athbdg=L1200&amp;from=/search</t>
   </si>
   <si>
-    <t>Calories</t>
-  </si>
-  <si>
     <t>https://www.walmart.com/ip/Great-Value-Ground-Black-Pepper-6-oz/44662571?athbdg=L1600&amp;from=/search</t>
   </si>
   <si>
@@ -708,6 +705,9 @@
   </si>
   <si>
     <t>loaf</t>
+  </si>
+  <si>
+    <t>calories</t>
   </si>
 </sst>
 </file>
@@ -1052,7 +1052,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomRight" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1099,7 +1099,7 @@
         <v>69</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>178</v>
+        <v>223</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>30</v>
@@ -1116,7 +1116,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D2">
         <v>10</v>
@@ -1125,7 +1125,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
@@ -1135,7 +1135,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G3" s="1">
         <v>1</v>
@@ -1151,13 +1151,13 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I4" s="1">
         <v>1</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -1167,7 +1167,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K5" s="1">
         <v>1</v>
@@ -1424,13 +1424,13 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B15" t="s">
         <v>99</v>
       </c>
       <c r="C15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D15" s="2">
         <v>0.27</v>
@@ -1540,13 +1540,13 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B20" t="s">
         <v>99</v>
       </c>
       <c r="C20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D20" s="2">
         <v>3.48</v>
@@ -2029,7 +2029,7 @@
         <v>129</v>
       </c>
       <c r="C36" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D36" s="2">
         <v>1.1200000000000001</v>
@@ -2038,10 +2038,10 @@
         <v>0.5</v>
       </c>
       <c r="F36" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="P36" t="s">
         <v>180</v>
-      </c>
-      <c r="P36" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
@@ -2084,7 +2084,7 @@
         <v>129</v>
       </c>
       <c r="C38" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D38" s="2">
         <v>5.64</v>
@@ -2093,10 +2093,10 @@
         <v>1</v>
       </c>
       <c r="F38" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="P38" t="s">
         <v>180</v>
-      </c>
-      <c r="P38" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
@@ -2107,7 +2107,7 @@
         <v>129</v>
       </c>
       <c r="C39" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D39" s="2">
         <v>2.2400000000000002</v>
@@ -2116,10 +2116,10 @@
         <v>0.5</v>
       </c>
       <c r="F39" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="P39" t="s">
         <v>180</v>
-      </c>
-      <c r="P39" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
@@ -2130,7 +2130,7 @@
         <v>129</v>
       </c>
       <c r="C40" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D40" s="2">
         <v>1.1200000000000001</v>
@@ -2139,10 +2139,10 @@
         <v>0.5</v>
       </c>
       <c r="F40" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="P40" t="s">
         <v>180</v>
-      </c>
-      <c r="P40" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
@@ -2153,7 +2153,7 @@
         <v>129</v>
       </c>
       <c r="C41" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D41" s="2">
         <v>1.1200000000000001</v>
@@ -2162,10 +2162,10 @@
         <v>0.5</v>
       </c>
       <c r="F41" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="P41" t="s">
         <v>180</v>
-      </c>
-      <c r="P41" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
@@ -2176,7 +2176,7 @@
         <v>129</v>
       </c>
       <c r="C42" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D42" s="2">
         <v>1.1200000000000001</v>
@@ -2185,10 +2185,10 @@
         <v>0.5</v>
       </c>
       <c r="F42" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="P42" t="s">
         <v>180</v>
-      </c>
-      <c r="P42" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
@@ -2208,7 +2208,7 @@
         <v>129</v>
       </c>
       <c r="C44" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D44" s="2">
         <v>1.1200000000000001</v>
@@ -2217,10 +2217,10 @@
         <v>0.5</v>
       </c>
       <c r="F44" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="P44" t="s">
         <v>180</v>
-      </c>
-      <c r="P44" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
@@ -2231,7 +2231,7 @@
         <v>129</v>
       </c>
       <c r="C45" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D45" s="2">
         <v>3.98</v>
@@ -2240,10 +2240,10 @@
         <v>1</v>
       </c>
       <c r="F45" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="P45" t="s">
         <v>180</v>
-      </c>
-      <c r="P45" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
@@ -2254,7 +2254,7 @@
         <v>129</v>
       </c>
       <c r="C46" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D46" s="2">
         <v>1.28</v>
@@ -2263,10 +2263,10 @@
         <v>0.5</v>
       </c>
       <c r="F46" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="P46" t="s">
         <v>180</v>
-      </c>
-      <c r="P46" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
@@ -2277,7 +2277,7 @@
         <v>129</v>
       </c>
       <c r="C47" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D47" s="2">
         <v>1.1200000000000001</v>
@@ -2286,10 +2286,10 @@
         <v>0.5</v>
       </c>
       <c r="F47" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="P47" t="s">
         <v>180</v>
-      </c>
-      <c r="P47" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
@@ -2309,10 +2309,10 @@
         <v>0.5</v>
       </c>
       <c r="F48" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="P48" t="s">
         <v>180</v>
-      </c>
-      <c r="P48" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
@@ -2323,7 +2323,7 @@
         <v>129</v>
       </c>
       <c r="C49" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D49" s="2">
         <v>3.78</v>
@@ -2332,10 +2332,10 @@
         <v>0.5</v>
       </c>
       <c r="F49" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="P49" t="s">
         <v>180</v>
-      </c>
-      <c r="P49" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
@@ -2346,7 +2346,7 @@
         <v>129</v>
       </c>
       <c r="C50" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D50" s="2">
         <v>2.42</v>
@@ -2355,21 +2355,21 @@
         <v>0.5</v>
       </c>
       <c r="F50" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="P50" t="s">
         <v>180</v>
-      </c>
-      <c r="P50" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B51" t="s">
         <v>129</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D51" s="2">
         <v>0.89</v>
@@ -2788,7 +2788,7 @@
         <v>166</v>
       </c>
       <c r="C64" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D64" s="2">
         <v>13.99</v>
@@ -2797,7 +2797,7 @@
         <v>144</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L64">
         <v>1872</v>
@@ -3369,7 +3369,7 @@
         <v>172</v>
       </c>
       <c r="C86" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D86" s="2">
         <v>3.24</v>
@@ -3465,7 +3465,7 @@
         <v>176</v>
       </c>
       <c r="C89" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D89" s="2">
         <v>1.5</v>
@@ -3491,10 +3491,10 @@
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
+        <v>191</v>
+      </c>
+      <c r="C90" t="s">
         <v>192</v>
-      </c>
-      <c r="C90" t="s">
-        <v>193</v>
       </c>
       <c r="D90" s="2">
         <v>4.28</v>
@@ -3520,34 +3520,34 @@
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B91" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D91" s="2"/>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B92" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D92" s="2"/>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B93" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D93" s="2"/>
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B94" t="s">
         <v>176</v>
@@ -3576,13 +3576,13 @@
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B95" t="s">
         <v>167</v>
       </c>
       <c r="C95" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D95" s="2">
         <v>1.99</v>
@@ -3608,13 +3608,13 @@
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B96" t="s">
         <v>171</v>
       </c>
       <c r="C96" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D96" s="2">
         <v>2.99</v>
@@ -3637,13 +3637,13 @@
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B97" t="s">
         <v>176</v>
       </c>
       <c r="C97" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D97" s="2">
         <v>3.98</v>
@@ -3675,13 +3675,13 @@
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B98" t="s">
         <v>171</v>
       </c>
       <c r="C98" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D98" s="2">
         <v>1.47</v>

</xml_diff>